<commit_message>
type email dans le formulaire
</commit_message>
<xml_diff>
--- a/Modele-audit-SEO.xlsx
+++ b/Modele-audit-SEO.xlsx
@@ -115,7 +115,7 @@
     <t xml:space="preserve">http://www.seo-reference.net/optimisation/texte-cache.html</t>
   </si>
   <si>
-    <t xml:space="preserve">Du texte est caché</t>
+    <t xml:space="preserve">Du texte est caché sur la page de contact</t>
   </si>
   <si>
     <t xml:space="preserve">Le texte n’est pas visible</t>
@@ -501,8 +501,8 @@
   </sheetPr>
   <dimension ref="A1:Z23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A17" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E21" activeCellId="0" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -720,8 +720,7 @@
         <v>37</v>
       </c>
       <c r="E10" s="5" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F10" s="7" t="s">
         <v>16</v>
@@ -920,7 +919,7 @@
         <v>74</v>
       </c>
       <c r="E20" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F20" s="7" t="s">
         <v>60</v>

</xml_diff>